<commit_message>
Updated Test Plan for LibraryItem class excel file.
</commit_message>
<xml_diff>
--- a/tests/test_plan_library_item.xlsx
+++ b/tests/test_plan_library_item.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lauri\Desktop\Intermediate Software Development0315\8. Activities\Module_01\given_files\activity_1\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Trieu\Documents\rrc-polytech\ADD\Semester-2\intermediate_software_development\activities\activity_1\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94801D8B-F184-4C7C-AC17-1E2ABA18B123}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86EF043C-C485-43BD-92CB-EBF898A882DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -183,7 +183,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="34">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -249,6 +249,50 @@
   </si>
   <si>
     <t>Attribute  set to input values.</t>
+  </si>
+  <si>
+    <t>Tri Tranvo</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>title = "Hobbit"
+author = "Tolkien"
+genre = "FANTASY"</t>
+  </si>
+  <si>
+    <t>title = ""
+author = "Tolkien"
+genre = "FANTASY"</t>
+  </si>
+  <si>
+    <t>title = "Hobbit"
+author = ""
+genre = "FANTASY"</t>
+  </si>
+  <si>
+    <t>title = "Hobbit"
+author = "Tolkien"
+genre = Invalid</t>
+  </si>
+  <si>
+    <t>Attributes set</t>
+  </si>
+  <si>
+    <t>ValueError</t>
+  </si>
+  <si>
+    <t>LibraryItem("Hobbit", "Tolkien", "FANTASY")</t>
+  </si>
+  <si>
+    <t>Hobbit</t>
+  </si>
+  <si>
+    <t>Tolkien</t>
+  </si>
+  <si>
+    <t>FANTASY</t>
   </si>
 </sst>
 </file>
@@ -1109,8 +1153,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DADEBCC4-BB44-48CD-B9AB-1E2FD3EE0EEB}">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1140,7 +1184,9 @@
       <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="15"/>
+      <c r="C3" s="15" t="s">
+        <v>22</v>
+      </c>
       <c r="D3" s="16"/>
     </row>
     <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1186,9 +1232,15 @@
       <c r="D7" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
+      <c r="E7" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="8" spans="1:7" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
@@ -1201,9 +1253,15 @@
       <c r="D8" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
+      <c r="E8" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
@@ -1216,9 +1274,15 @@
       <c r="D9" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
+      <c r="E9" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="10" spans="1:7" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
@@ -1231,9 +1295,15 @@
       <c r="D10" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
+      <c r="E10" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="11" spans="1:7" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="12">
@@ -1245,9 +1315,15 @@
       <c r="D11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
+      <c r="E11" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="12" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="12">
@@ -1259,9 +1335,15 @@
       <c r="D12" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
+      <c r="E12" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="13" spans="1:7" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="11">
@@ -1273,9 +1355,15 @@
       <c r="D13" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
+      <c r="E13" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="14" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="11">
@@ -1413,6 +1501,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003B3B6B51C940774DBF92367B1D1A75F0" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="80d4f13eaa95653e2ff902bb880fefc3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ee0e594b-5dc6-49aa-9be8-f17bb89b127c" xmlns:ns3="b80edf0c-bd47-4bae-8c19-89fc2af9398f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6ababe2f621e4b192c84b1cec6edec4f" ns2:_="" ns3:_="">
     <xsd:import namespace="ee0e594b-5dc6-49aa-9be8-f17bb89b127c"/>
@@ -1607,15 +1704,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1628,13 +1716,39 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37F01E9C-39D8-491B-950E-769C54FF39B2}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3194B8C0-471E-4E12-8338-7B9268783B6C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3194B8C0-471E-4E12-8338-7B9268783B6C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37F01E9C-39D8-491B-950E-769C54FF39B2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="ee0e594b-5dc6-49aa-9be8-f17bb89b127c"/>
+    <ds:schemaRef ds:uri="b80edf0c-bd47-4bae-8c19-89fc2af9398f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{93494D4A-B25F-4AE9-9242-3524F3518EDF}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{93494D4A-B25F-4AE9-9242-3524F3518EDF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ee0e594b-5dc6-49aa-9be8-f17bb89b127c"/>
+    <ds:schemaRef ds:uri="b80edf0c-bd47-4bae-8c19-89fc2af9398f"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated Test Plan with entries related to the new attributes for LibraryItem class.
</commit_message>
<xml_diff>
--- a/tests/test_plan_library_item.xlsx
+++ b/tests/test_plan_library_item.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Trieu\Documents\rrc-polytech\ADD\Semester-2\intermediate_software_development\activities\activity_1\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86EF043C-C485-43BD-92CB-EBF898A882DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82FAD6F0-C556-46ED-B250-528BA37A7180}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -183,7 +183,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="42">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -257,49 +257,89 @@
     <t>None</t>
   </si>
   <si>
-    <t>title = "Hobbit"
+    <t>Attributes set</t>
+  </si>
+  <si>
+    <t>ValueError</t>
+  </si>
+  <si>
+    <t>Hobbit</t>
+  </si>
+  <si>
+    <t>Tolkien</t>
+  </si>
+  <si>
+    <t>FANTASY</t>
+  </si>
+  <si>
+    <t>Exception raised when item_id is non numeric</t>
+  </si>
+  <si>
+    <t>Exception raised when is_borrowed is not boolean</t>
+  </si>
+  <si>
+    <t>item_id</t>
+  </si>
+  <si>
+    <t>is_borrowed</t>
+  </si>
+  <si>
+    <t>returns item_id attribute</t>
+  </si>
+  <si>
+    <t>returns is_borrowed attribute</t>
+  </si>
+  <si>
+    <t>LibraryItem(777 ,"Hobbit", "Tolkien", "FANTASY", FALSE)</t>
+  </si>
+  <si>
+    <t>item_id = 777
+title = "Hobbit"
 author = "Tolkien"
-genre = "FANTASY"</t>
-  </si>
-  <si>
-    <t>title = ""
+genre = INVALID
+is_borrowed = FALSE</t>
+  </si>
+  <si>
+    <t>item_id = 777
+title = "Hobbit"
+author = "   "
+genre = FANTASY
+is_borrowed = FALSE</t>
+  </si>
+  <si>
+    <t>item_id = 777
+title = "Hobbit"
 author = "Tolkien"
-genre = "FANTASY"</t>
-  </si>
-  <si>
-    <t>title = "Hobbit"
-author = ""
-genre = "FANTASY"</t>
-  </si>
-  <si>
-    <t>title = "Hobbit"
+genre = FANTASY
+is_borrowed = FALSE</t>
+  </si>
+  <si>
+    <t>item_id = 777
+title = "   "
 author = "Tolkien"
-genre = Invalid</t>
-  </si>
-  <si>
-    <t>Attributes set</t>
-  </si>
-  <si>
-    <t>ValueError</t>
-  </si>
-  <si>
-    <t>LibraryItem("Hobbit", "Tolkien", "FANTASY")</t>
-  </si>
-  <si>
-    <t>Hobbit</t>
-  </si>
-  <si>
-    <t>Tolkien</t>
-  </si>
-  <si>
-    <t>FANTASY</t>
+genre = FANTASY
+is_borrowed = FALSE</t>
+  </si>
+  <si>
+    <t>item_id = "777"
+title = "Hobbit"
+author = "Tolkien"
+genre = FANTASY
+is_borrowed = FALSE</t>
+  </si>
+  <si>
+    <t>item_id = 777
+title = "Hobbit"
+author = "Tolkien"
+genre = FANTASY
+is_borrowed = MAYBE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -360,6 +400,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -547,7 +595,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -596,6 +644,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" shrinkToFit="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -827,8 +890,8 @@
     <tableColumn id="2" xr3:uid="{1904C92F-9639-4229-AA4E-4C4DEAF21EEE}" name="Method being Tested" dataDxfId="4"/>
     <tableColumn id="3" xr3:uid="{4E480EB6-99FB-4F51-98B5-D5BE13327E8C}" name="Condition being Tested" dataDxfId="3"/>
     <tableColumn id="4" xr3:uid="{5381561B-09C5-439D-999E-CD8E013F9561}" name="Preconditions" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{645704DE-22F5-4239-BEB6-F4252A1F2823}" name="Method Inputs" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{101F480E-86C3-4E60-AA1E-2FCAD389E35F}" name="Expected Result" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{645704DE-22F5-4239-BEB6-F4252A1F2823}" name="Method Inputs" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{101F480E-86C3-4E60-AA1E-2FCAD389E35F}" name="Expected Result" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1151,10 +1214,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DADEBCC4-BB44-48CD-B9AB-1E2FD3EE0EEB}">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1163,12 +1226,12 @@
     <col min="3" max="3" width="22.28515625" customWidth="1"/>
     <col min="4" max="4" width="32.7109375" customWidth="1"/>
     <col min="5" max="5" width="29.140625" customWidth="1"/>
-    <col min="6" max="6" width="35.42578125" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="26.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:7" ht="73.150000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="1.45">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:10" ht="73.150000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="1.45">
       <c r="B2" s="2" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
@@ -1180,7 +1243,7 @@
       <c r="F2" s="14"/>
       <c r="G2" s="14"/>
     </row>
-    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
@@ -1189,7 +1252,7 @@
       </c>
       <c r="D3" s="16"/>
     </row>
-    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="6" t="s">
         <v>3</v>
       </c>
@@ -1198,10 +1261,10 @@
       </c>
       <c r="D4" s="18"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="7" t="s">
         <v>0</v>
       </c>
@@ -1221,7 +1284,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="78" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="78" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="11">
         <v>1</v>
@@ -1235,14 +1298,14 @@
       <c r="E7" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="F7" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="G7" s="9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:10" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="12">
         <v>2</v>
@@ -1256,14 +1319,14 @@
       <c r="E8" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F8" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="G8" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:10" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="12">
         <v>3</v>
@@ -1277,14 +1340,14 @@
       <c r="E9" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F9" s="9" t="s">
-        <v>26</v>
+      <c r="F9" s="23" t="s">
+        <v>37</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="11">
         <v>4</v>
@@ -1298,14 +1361,14 @@
       <c r="E10" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="9" t="s">
-        <v>27</v>
+      <c r="F10" s="23" t="s">
+        <v>36</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="12">
         <v>5</v>
       </c>
@@ -1316,16 +1379,16 @@
         <v>17</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="F11" s="9" t="s">
         <v>23</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="12">
         <v>6</v>
       </c>
@@ -1336,16 +1399,16 @@
         <v>18</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="F12" s="9" t="s">
         <v>23</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="11">
         <v>7</v>
       </c>
@@ -1356,54 +1419,91 @@
         <v>19</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="F13" s="9" t="s">
         <v>23</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="11">
         <v>10</v>
       </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
+      <c r="C14" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" s="25" t="s">
+        <v>40</v>
+      </c>
       <c r="G14" s="3"/>
-    </row>
-    <row r="15" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J14" s="24"/>
+    </row>
+    <row r="15" spans="1:10" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="12">
         <v>11</v>
       </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
+      <c r="C15" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" s="23" t="s">
+        <v>41</v>
+      </c>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="12">
         <v>12</v>
       </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
+      <c r="C16" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G16" s="22">
+        <v>777</v>
+      </c>
     </row>
     <row r="17" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="11">
         <v>13</v>
       </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
+      <c r="C17" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G17" s="21" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="12">
@@ -1510,6 +1610,17 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ee0e594b-5dc6-49aa-9be8-f17bb89b127c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="b80edf0c-bd47-4bae-8c19-89fc2af9398f" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003B3B6B51C940774DBF92367B1D1A75F0" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="80d4f13eaa95653e2ff902bb880fefc3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ee0e594b-5dc6-49aa-9be8-f17bb89b127c" xmlns:ns3="b80edf0c-bd47-4bae-8c19-89fc2af9398f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6ababe2f621e4b192c84b1cec6edec4f" ns2:_="" ns3:_="">
     <xsd:import namespace="ee0e594b-5dc6-49aa-9be8-f17bb89b127c"/>
@@ -1704,17 +1815,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ee0e594b-5dc6-49aa-9be8-f17bb89b127c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="b80edf0c-bd47-4bae-8c19-89fc2af9398f" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3194B8C0-471E-4E12-8338-7B9268783B6C}">
   <ds:schemaRefs>
@@ -1724,6 +1824,17 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{93494D4A-B25F-4AE9-9242-3524F3518EDF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ee0e594b-5dc6-49aa-9be8-f17bb89b127c"/>
+    <ds:schemaRef ds:uri="b80edf0c-bd47-4bae-8c19-89fc2af9398f"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37F01E9C-39D8-491B-950E-769C54FF39B2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1740,15 +1851,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{93494D4A-B25F-4AE9-9242-3524F3518EDF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="ee0e594b-5dc6-49aa-9be8-f17bb89b127c"/>
-    <ds:schemaRef ds:uri="b80edf0c-bd47-4bae-8c19-89fc2af9398f"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>